<commit_message>
fix report acdc project & menu hrd
</commit_message>
<xml_diff>
--- a/app_wams/public/export/excel/laporan-DCL.xlsx
+++ b/app_wams/public/export/excel/laporan-DCL.xlsx
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
-  <si>
-    <t>Export Laporan Transaction Maker DCL Periode 01/Jan/23 - 31/Jan/23</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>Export Laporan Transaction Maker DCL Periode 01/Dec/22 - 31/Dec/22</t>
   </si>
   <si>
     <t>Project Name</t>
@@ -40,67 +40,28 @@
     <t>Tanggal Pengajuan</t>
   </si>
   <si>
-    <t>data telah di hapus</t>
-  </si>
-  <si>
-    <t>PT. MIB</t>
-  </si>
-  <si>
-    <t>Sinta</t>
-  </si>
-  <si>
-    <t>2023-01-18</t>
-  </si>
-  <si>
-    <t>PT. Amoro</t>
-  </si>
-  <si>
-    <t>Export Laporan Data DCL Periode 01/Jan/23 - 31/Jan/23</t>
+    <t>Export Laporan Data DCL Periode 01/Dec/22 - 31/Dec/22</t>
   </si>
   <si>
     <t>Total Nominal DCL</t>
   </si>
   <si>
-    <t>Rp18,000,000</t>
+    <t>Rp0</t>
   </si>
   <si>
     <t>Nama disti</t>
   </si>
   <si>
-    <t>SMI</t>
-  </si>
-  <si>
-    <t>BPT</t>
-  </si>
-  <si>
     <t>Pic disti</t>
   </si>
   <si>
-    <t>hana</t>
-  </si>
-  <si>
-    <t>hana2</t>
-  </si>
-  <si>
     <t>Jabatan pic</t>
   </si>
   <si>
-    <t>Manager</t>
-  </si>
-  <si>
     <t>Email pic</t>
   </si>
   <si>
-    <t>manager@mail.com</t>
-  </si>
-  <si>
     <t>Nomor hp</t>
-  </si>
-  <si>
-    <t>0988889231</t>
-  </si>
-  <si>
-    <t>09888892314</t>
   </si>
   <si>
     <t>Pengajuan cl</t>
@@ -457,7 +418,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2:F2"/>
@@ -500,42 +461,6 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3"/>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>9000000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4"/>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>500000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +487,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A4" sqref="A4:G4"/>
@@ -572,7 +497,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -583,79 +508,33 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5">
-        <v>9000000</v>
-      </c>
-      <c r="G5">
-        <v>9000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6">
-        <v>9000000</v>
-      </c>
-      <c r="G6">
-        <v>9000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>